<commit_message>
setup complete but item page needs some modificaton
</commit_message>
<xml_diff>
--- a/BipuniBitan_UI/Documentation/BipuniBitan(Desktop App)TimeLine.xlsx
+++ b/BipuniBitan_UI/Documentation/BipuniBitan(Desktop App)TimeLine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inventory Matrials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inventory Matrials\Desktop App\BipuniBitan_UI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="TimeLine" sheetId="1" r:id="rId1"/>
-    <sheet name="Setup form " sheetId="2" r:id="rId2"/>
+    <sheet name="Transaction" sheetId="2" r:id="rId2"/>
+    <sheet name="Setup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="93">
   <si>
     <t>Module Name</t>
   </si>
@@ -292,13 +293,25 @@
   </si>
   <si>
     <t>nvarchar(2000)</t>
+  </si>
+  <si>
+    <t>Pending task</t>
+  </si>
+  <si>
+    <t>Image save, retrieve need to folder, from folder</t>
+  </si>
+  <si>
+    <t>Transaction Page Name</t>
+  </si>
+  <si>
+    <t>Fields for Transaction page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +353,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -389,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -412,12 +432,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -427,6 +441,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,13 +770,15 @@
       <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -767,10 +795,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
+      <c r="B7" s="15"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
@@ -779,10 +807,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
+      <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
@@ -794,7 +822,7 @@
     <row r="12" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -803,59 +831,73 @@
       <c r="E14" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="F14" s="17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
+      <c r="B15" s="15"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="2:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="2:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="2:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
       <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-    </row>
-    <row r="20" spans="2:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="2:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="2:7" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
       <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="2:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="2:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="F22" s="17"/>
+    </row>
+    <row r="23" spans="2:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C27" t="s">
@@ -865,11 +907,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="16"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="16"/>
       <c r="C29" t="s">
         <v>27</v>
       </c>
@@ -877,11 +919,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="16"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="16"/>
       <c r="C31" t="s">
         <v>28</v>
       </c>
@@ -889,11 +931,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="16"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
+      <c r="B33" s="16"/>
       <c r="C33" t="s">
         <v>32</v>
       </c>
@@ -902,10 +944,10 @@
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
+      <c r="B34" s="16"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C38" t="s">
@@ -913,19 +955,19 @@
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
+      <c r="B39" s="16"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="11"/>
+      <c r="B40" s="16"/>
       <c r="C40" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
+      <c r="B41" s="16"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="11"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="9" t="s">
         <v>37</v>
       </c>
@@ -939,11 +981,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B14:B22"/>
     <mergeCell ref="B27:B34"/>
     <mergeCell ref="B38:B42"/>
+    <mergeCell ref="F14:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -954,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,21 +1010,21 @@
     <col min="6" max="6" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+    <row r="1" spans="1:2" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -995,8 +1038,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1020,13 +1063,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
+    <row r="19" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1040,8 +1083,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+    <row r="27" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1095,8 +1138,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+    <row r="40" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1119,16 +1162,16 @@
       <c r="B44" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="12" t="s">
+      <c r="G44" s="10" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1136,13 +1179,13 @@
       <c r="B45" t="s">
         <v>53</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="G45" s="10" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1150,13 +1193,13 @@
       <c r="B46" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="G46" s="10" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1164,13 +1207,13 @@
       <c r="B47" t="s">
         <v>55</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G47" s="12" t="s">
+      <c r="G47" s="10" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1178,119 +1221,119 @@
       <c r="B48" t="s">
         <v>56</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G48" s="12" t="s">
+      <c r="G48" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="49" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G49" s="12" t="s">
+      <c r="G49" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="50" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G50" s="12" t="s">
+      <c r="G50" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="51" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F51" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G51" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="52" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G52" s="12" t="s">
+      <c r="G52" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E53" s="12" t="s">
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E53" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G53" s="12" t="s">
+      <c r="G53" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="G54" s="12" t="s">
+      <c r="G54" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E55" s="12" t="s">
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E55" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G55" s="12" t="s">
+      <c r="G55" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E56" s="12" t="s">
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E56" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="G56" s="12" t="s">
+      <c r="G56" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E57" s="12" t="s">
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E57" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G57" s="12" t="s">
+      <c r="G57" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="58" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12" t="s">
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1298,4 +1341,353 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.375" customWidth="1"/>
+    <col min="2" max="2" width="36.125" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="29.125" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E49" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E50" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E51" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E52" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E53" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E54" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E55" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E56" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E57" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>